<commit_message>
Classwork + tutor's HW
</commit_message>
<xml_diff>
--- a/38_Tables_2/homework/18_1.xlsx
+++ b/38_Tables_2/homework/18_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub repos\ICT_EGE\38_Tables_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub repos\ICT_EGE\38_Tables_2\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F907F50D-C8FB-4772-8196-B1369D34C74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4C586D-51ED-49B3-97D7-093AAA767E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,10 +29,30 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>МАКС</t>
+  </si>
+  <si>
+    <t>МИН</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -153,6 +173,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -433,13 +454,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="19" max="19" width="3" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
@@ -995,6 +1019,7 @@
       <c r="N11" s="7">
         <v>31</v>
       </c>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1039,6 +1064,7 @@
       <c r="N12" s="7">
         <v>61</v>
       </c>
+      <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1083,6 +1109,13 @@
       <c r="N13" s="7">
         <v>78</v>
       </c>
+      <c r="R13" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1"/>
+      <c r="T13" s="11" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
@@ -1127,6 +1160,7 @@
       <c r="N14" s="10">
         <v>17</v>
       </c>
+      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
@@ -1138,6 +1172,13 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>